<commit_message>
Done with 595. Big Countries
</commit_message>
<xml_diff>
--- a/SQL_StudyPlan/SQL_1/ProbList.xlsx
+++ b/SQL_StudyPlan/SQL_1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -51,13 +51,31 @@
   </si>
   <si>
     <t>Understanding</t>
+  </si>
+  <si>
+    <t>Big Countries</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t>❌</t>
+  </si>
+  <si>
+    <t>Given 2 sol and didn’t see solutions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +91,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +109,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,12 +146,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,18 +437,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -444,7 +480,36 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>595</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done with 1757. Recyclable and Low Fat Products
</commit_message>
<xml_diff>
--- a/SQL_StudyPlan/SQL_1/ProbList.xlsx
+++ b/SQL_StudyPlan/SQL_1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>No.</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Given 2 sol and didn’t see solutions</t>
+  </si>
+  <si>
+    <t>Recyclable and Low Fat Products</t>
   </si>
 </sst>
 </file>
@@ -437,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="23.140625" style="4" customWidth="1"/>
@@ -455,7 +458,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -484,7 +487,7 @@
       <c r="A2" s="5">
         <v>595</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -503,8 +506,91 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1757</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
       <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done with 584. Find Customer Referee
</commit_message>
<xml_diff>
--- a/SQL_StudyPlan/SQL_1/ProbList.xlsx
+++ b/SQL_StudyPlan/SQL_1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>No.</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Main Topic</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
     <t>Related Topics</t>
   </si>
   <si>
@@ -72,6 +69,12 @@
   </si>
   <si>
     <t>Recyclable and Low Fat Products</t>
+  </si>
+  <si>
+    <t>Find Customer Referee</t>
+  </si>
+  <si>
+    <t>Given 1 sol and didn’t see solutions</t>
   </si>
 </sst>
 </file>
@@ -440,21 +443,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +470,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -476,122 +479,137 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>595</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1757</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>584</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H16" s="3" t="s">
-        <v>13</v>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done with 183. Find Customer Referee
</commit_message>
<xml_diff>
--- a/SQL_StudyPlan/SQL_1/ProbList.xlsx
+++ b/SQL_StudyPlan/SQL_1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>No.</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Given 1 sol and didn’t see solutions</t>
+  </si>
+  <si>
+    <t>Customers Who Never Order</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -163,6 +166,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +450,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,9 +556,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>183</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 1873. Calculate Special Bonus
</commit_message>
<xml_diff>
--- a/SQL_StudyPlan/SQL_1/ProbList.xlsx
+++ b/SQL_StudyPlan/SQL_1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>No.</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Customers Who Never Order</t>
+  </si>
+  <si>
+    <t>Calculate Special Bonus</t>
+  </si>
+  <si>
+    <t>SELECT and ORDER</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,13 +456,13 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="23.140625" style="4" customWidth="1"/>
   </cols>
@@ -468,7 +474,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -494,7 +500,7 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
@@ -517,7 +523,7 @@
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
@@ -540,7 +546,7 @@
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
@@ -563,7 +569,7 @@
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
@@ -579,9 +585,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1873</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with 627. Swap Salary
</commit_message>
<xml_diff>
--- a/SQL_StudyPlan/SQL_1/ProbList.xlsx
+++ b/SQL_StudyPlan/SQL_1/ProbList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>No.</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>SELECT and ORDER</t>
+  </si>
+  <si>
+    <t>Swap Salary</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>Copied 1 sol from sols and understood</t>
   </si>
 </sst>
 </file>
@@ -456,7 +465,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +617,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>627</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>